<commit_message>
changed example paths for easier testing from random usb stick
</commit_message>
<xml_diff>
--- a/published/list of documents.xlsx
+++ b/published/list of documents.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22998" windowHeight="4200"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10416"/>
   </bookViews>
   <sheets>
     <sheet name="DocumentList" sheetId="2" r:id="rId1"/>
@@ -172,31 +172,31 @@
     <t>Package II Category I 2</t>
   </si>
   <si>
-    <t>E:/Quality Management/published/Another Process Instruction .pdf</t>
-  </si>
-  <si>
-    <t>E:/Quality Management/published/Another Sample Form.pdf</t>
-  </si>
-  <si>
-    <t>E:/Quality Management/published/Attendance List.pdf</t>
-  </si>
-  <si>
-    <t>E:/Quality Management/published/Having Several Dozen Documents Making This System Plausible.pdf</t>
-  </si>
-  <si>
-    <t>E:/Quality Management/published/Sample Form.pdf</t>
-  </si>
-  <si>
-    <t>E:/Quality Management/published/Protocol.pdf</t>
-  </si>
-  <si>
-    <t>E:/Quality Management/published/Process Instruction.pdf</t>
-  </si>
-  <si>
-    <t>E:/Quality Management/published/Find This File Searching For Something That Rhymes With COOL.pdf</t>
-  </si>
-  <si>
-    <t>E:/Quality Management/published/Interactive dynamic DOCM.docm</t>
+    <t>D:/Quality Management/published/Another Process Instruction .pdf</t>
+  </si>
+  <si>
+    <t>D:/Quality Management/published/Another Sample Form.pdf</t>
+  </si>
+  <si>
+    <t>D:/Quality Management/published/Attendance List.pdf</t>
+  </si>
+  <si>
+    <t>D:/Quality Management/published/Having Several Dozen Documents Making This System Plausible.pdf</t>
+  </si>
+  <si>
+    <t>D:/Quality Management/published/Sample Form.pdf</t>
+  </si>
+  <si>
+    <t>D:/Quality Management/published/Protocol.pdf</t>
+  </si>
+  <si>
+    <t>D:/Quality Management/published/Process Instruction.pdf</t>
+  </si>
+  <si>
+    <t>D:/Quality Management/published/Find This File Searching For Something That Rhymes With COOL.pdf</t>
+  </si>
+  <si>
+    <t>D:/Quality Management/published/Interactive dynamic DOCM.docm</t>
   </si>
 </sst>
 </file>

</xml_diff>